<commit_message>
cleaned the description bit
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="619">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -59,7 +59,7 @@
     <t xml:space="preserve"> UK , USA </t>
   </si>
   <si>
-    <t xml:space="preserve"> 361,300,000        
+    <t xml:space="preserve"> 361,400,000        
         </t>
   </si>
   <si>
@@ -181,6 +181,9 @@
     <t xml:space="preserve"> girl, female protagonist, disney plus, christmas, </t>
   </si>
   <si>
+    <t xml:space="preserve"> Comedy, Drama, Family, Fantasy</t>
+  </si>
+  <si>
     <t xml:space="preserve">
  The Montecito Picture Company, Walt Disney Pictures      
         </t>
@@ -228,7 +231,7 @@
     <t xml:space="preserve"> USA , Canada </t>
   </si>
   <si>
-    <t xml:space="preserve"> 1,028,979        
+    <t xml:space="preserve"> 1,401,954        
         </t>
   </si>
   <si>
@@ -246,7 +249,7 @@
     <t xml:space="preserve">Kate Pierce, now a cynical teen, is unexpectedly reunited with Santa Claus when a mysterious troublemaker threatens to cancel Christmas - forever.</t>
   </si>
   <si>
-    <t xml:space="preserve">Genres: Adventure, Comedy, Family, Fantasy</t>
+    <t xml:space="preserve"> Adventure, Comedy, Family, Fantasy</t>
   </si>
   <si>
     <t xml:space="preserve"> Canada </t>
@@ -272,7 +275,7 @@
     <t xml:space="preserve"> Action, Crime, Drama, Romance, Thriller</t>
   </si>
   <si>
-    <t xml:space="preserve"> 28,671,530        
+    <t xml:space="preserve"> 28,821,301        
         </t>
   </si>
   <si>
@@ -296,7 +299,7 @@
     <t xml:space="preserve"> Comedy, Horror, Thriller</t>
   </si>
   <si>
-    <t xml:space="preserve"> 14,194,365        
+    <t xml:space="preserve"> 14,179,080        
         </t>
   </si>
   <si>
@@ -338,6 +341,9 @@
     <t xml:space="preserve"> scientist, </t>
   </si>
   <si>
+    <t xml:space="preserve"> Drama, Fantasy, Sci-Fi, Thriller</t>
+  </si>
+  <si>
     <t xml:space="preserve">
  Anonymous Content, Netflix, Smokehouse Pictures      
         </t>
@@ -382,6 +388,9 @@
     <t xml:space="preserve"> holiday, christmas, </t>
   </si>
   <si>
+    <t xml:space="preserve"> Family, Fantasy, Musical</t>
+  </si>
+  <si>
     <t xml:space="preserve">
  Golden Girl, Get Lifted Film Company, 260 Degrees Entertainment      
         </t>
@@ -396,10 +405,13 @@
     <t xml:space="preserve"> fighting, christmas, santa claus, </t>
   </si>
   <si>
+    <t xml:space="preserve"> Action, Comedy, Fantasy, Thriller</t>
+  </si>
+  <si>
     <t xml:space="preserve"> UK , Canada , USA </t>
   </si>
   <si>
-    <t xml:space="preserve"> 1,028,657        
+    <t xml:space="preserve"> 1,082,179        
         </t>
   </si>
   <si>
@@ -437,6 +449,9 @@
     <t xml:space="preserve"> death, </t>
   </si>
   <si>
+    <t xml:space="preserve"> Thriller</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Canada , USA </t>
   </si>
   <si>
@@ -471,7 +486,7 @@
     <t xml:space="preserve">Black Bear</t>
   </si>
   <si>
-    <t xml:space="preserve">A filmmaker at a creative impasse seeks solace from her tumultuous past at a rural retreat, only to find that the woods summon her inner demons in intense and surprising ways.</t>
+    <t xml:space="preserve">At a remote lake house in the Adirondack Mountains, a couple entertains an out-of-town guest looking for inspiration in her filmmaking. The group quickly falls into a calculated game of desire, manipulation, and jealousy, unaware of how dangerously convoluted their lives will soon become in the filmmaker's pursuit of a work of art, which blurs the boundaries between autobiography and invention.</t>
   </si>
   <si>
     <t xml:space="preserve"> woods, interracial kiss, </t>
@@ -539,6 +554,9 @@
     <t xml:space="preserve"> author, cruise, aunt, nephew, </t>
   </si>
   <si>
+    <t xml:space="preserve"> Comedy, Drama</t>
+  </si>
+  <si>
     <t xml:space="preserve">
  Extension 765, HBO Films, LS Productions      
         </t>
@@ -556,6 +574,9 @@
     <t xml:space="preserve"> time travel, present, police officer, police officer hacked, police officer killed, </t>
   </si>
   <si>
+    <t xml:space="preserve"> Crime, Horror, Mystery, Thriller</t>
+  </si>
+  <si>
     <t xml:space="preserve"> South Korea </t>
   </si>
   <si>
@@ -576,7 +597,7 @@
     <t xml:space="preserve"> UK </t>
   </si>
   <si>
-    <t xml:space="preserve"> 25,919,223        
+    <t xml:space="preserve"> 26,287,085        
         </t>
   </si>
   <si>
@@ -597,9 +618,6 @@
     <t xml:space="preserve"> 1970s, uncle niece relationship, gay couple relationship, jewish lesbian, gay muslim, </t>
   </si>
   <si>
-    <t xml:space="preserve"> Comedy, Drama</t>
-  </si>
-  <si>
     <t xml:space="preserve">
  Amazon Studios, Miramax Films, Your Face Goes Here Entertainment      
         </t>
@@ -611,7 +629,7 @@
     <t xml:space="preserve">The 2nd</t>
   </si>
   <si>
-    <t xml:space="preserve">Secret-service agent Vic Davis is on his way to pick up his estranged son, Sean, from his college campus when he finds himself in the middle of a high-stakes terrorist operation. His son's friend Erin Walton, the daughter of Supreme Court Justice Walton is the target, and this armed faction will stop at nothing to kidnap her and use her as leverage for a pending landmark legal case.</t>
+    <t xml:space="preserve">Special forces agent Vic Davis is on his way to pick up his estranged son, Sean, from his college campus when he finds himself in the middle of a high-stakes terrorist operation. His son's friend Erin Walton, the daughter of Supreme Court Justice Walton is the target, and this armed faction will stop at nothing to kidnap her and use her as leverage for a pending landmark legal case.</t>
   </si>
   <si>
     <t xml:space="preserve"> secret agent, electronic music score, 2020s, 2010s, ambiguous ending, </t>
@@ -692,7 +710,7 @@
     <t xml:space="preserve"> Action, Horror, Sci-Fi</t>
   </si>
   <si>
-    <t xml:space="preserve"> 46,316,464        
+    <t xml:space="preserve"> 46,378,380        
         </t>
   </si>
   <si>
@@ -707,7 +725,7 @@
     <t xml:space="preserve">A 16 year-old girl returns home from camp and learns that her mother has a new boyfriend, one she intends to marry; a man whose charm, intelligence and beauty make him look like he's not human at all.</t>
   </si>
   <si>
-    <t xml:space="preserve">Genres: Horror, Mystery, Sci-Fi, Thriller</t>
+    <t xml:space="preserve"> Horror, Mystery, Sci-Fi, Thriller</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -752,13 +770,10 @@
     <t xml:space="preserve"> woke, live action cgi hybrid, ship, voyage, queen victoria, </t>
   </si>
   <si>
-    <t xml:space="preserve"> Adventure, Comedy, Family, Fantasy</t>
-  </si>
-  <si>
     <t xml:space="preserve"> USA , China , UK , Japan </t>
   </si>
   <si>
-    <t xml:space="preserve"> 245,231,781        
+    <t xml:space="preserve"> 246,073,367        
         </t>
   </si>
   <si>
@@ -782,7 +797,7 @@
     <t xml:space="preserve"> Crime, Drama, Thriller</t>
   </si>
   <si>
-    <t xml:space="preserve"> 10,133,050        
+    <t xml:space="preserve"> 10,136,930        
         </t>
   </si>
   <si>
@@ -800,6 +815,9 @@
     <t xml:space="preserve"> australian robots, australian horror, australian science fiction, </t>
   </si>
   <si>
+    <t xml:space="preserve"> Sci-Fi</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Australia </t>
   </si>
   <si>
@@ -864,7 +882,7 @@
     <t xml:space="preserve"> Ireland , UK </t>
   </si>
   <si>
-    <t xml:space="preserve"> 100,466        
+    <t xml:space="preserve"> 95,360        
         </t>
   </si>
   <si>
@@ -879,7 +897,7 @@
     <t xml:space="preserve">In 2024 a pandemic ravages the world and its cities. Centering on a handful of people as they navigate the obstacles currently hindering society: disease, martial law, quarantine, and vigilantes.</t>
   </si>
   <si>
-    <t xml:space="preserve"> reference to the coronavirus, male nudity, male rear nudity, shower, 2020, </t>
+    <t xml:space="preserve"> reference to the coronavirus, 2020, older man younger woman kiss, older man younger woman affair, produced by michael bay, </t>
   </si>
   <si>
     <t xml:space="preserve"> Comedy, Drama, Romance, Thriller</t>
@@ -919,7 +937,7 @@
     <t xml:space="preserve"> Animation, Adventure, Comedy, Family, Fantasy</t>
   </si>
   <si>
-    <t xml:space="preserve"> 76,344,105        
+    <t xml:space="preserve"> 76,631,640        
         </t>
   </si>
   <si>
@@ -943,7 +961,7 @@
     <t xml:space="preserve"> Canada , UK </t>
   </si>
   <si>
-    <t xml:space="preserve"> 872,555        
+    <t xml:space="preserve"> 883,546        
         </t>
   </si>
   <si>
@@ -1019,7 +1037,10 @@
     <t xml:space="preserve"> hero, one word title, </t>
   </si>
   <si>
-    <t xml:space="preserve"> 55,700        
+    <t xml:space="preserve"> Action, Adventure</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 54,570        
         </t>
   </si>
   <si>
@@ -1084,7 +1105,7 @@
     <t xml:space="preserve"> USA , Mexico , UK </t>
   </si>
   <si>
-    <t xml:space="preserve"> 19,000,000        
+    <t xml:space="preserve"> 22,100,000        
         </t>
   </si>
   <si>
@@ -1224,6 +1245,9 @@
     <t xml:space="preserve"> party, royalty, </t>
   </si>
   <si>
+    <t xml:space="preserve"> Comedy, Drama, Family, Romance</t>
+  </si>
+  <si>
     <t xml:space="preserve">
  Netflix, Motion Picture Corporation of America (MPCA), Brad Krevoy Television      
         </t>
@@ -1258,6 +1282,9 @@
     <t xml:space="preserve"> life, </t>
   </si>
   <si>
+    <t xml:space="preserve"> Comedy, Romance, Sci-Fi</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 1,600,000        
         </t>
   </si>
@@ -1291,7 +1318,7 @@
     <t xml:space="preserve">Neues aus der Welt</t>
   </si>
   <si>
-    <t xml:space="preserve">Five years after the end of the Civil War, Captain Jefferson Kyle Kidd (Tom Hanks), a veteran of three wars, now moves from town to town as a non-fiction storyteller, sharing the news of presidents and queens, glorious feuds, devastating catastrophes, and gripping adventures from the far reaches of the globe. In the plains of Texas, he crosses paths with Johanna (Helena Zengel ), a 10-year-old taken in by the Kiowa people six years earlier and raised as one of their own. Johanna, hostile to a world she's never experienced, is being returned to her biological aunt and uncle against her will. Kidd agrees to deliver the child where the law says she belongs. As they travel hundreds of miles into the unforgiving wilderness, the two will face tremendous challenges of both human and natural forces as they search for a place that either can call home.</t>
+    <t xml:space="preserve">Five years after the end of the Civil War, Captain Jefferson Kyle Kidd (Tom Hanks), a veteran of three wars, now moves from town to town as a non-fiction storyteller, sharing the news of presidents and queens, glorious feuds, devastating catastrophes, and gripping adventures from the far reaches of the globe. On the plains of Texas, he crosses paths with Johanna (Helena Zengel), a 10-year-old taken in by the Kiowa people six years earlier and raised as one of their own. Johanna, hostile to a world she's never experienced, is being returned to her biological aunt and uncle against her will. Kidd agrees to deliver the child where the law says she belongs. As they travel hundreds of miles into the unforgiving wilderness, the two will face tremendous challenges of both human and natural forces as they search for a place that either can call home.</t>
   </si>
   <si>
     <t xml:space="preserve"> 1800s, rescue, wild west, cowboy, spaghetti western, </t>
@@ -1305,6 +1332,9 @@
         </t>
   </si>
   <si>
+    <t xml:space="preserve"> 118 </t>
+  </si>
+  <si>
     <t xml:space="preserve">Rebecca</t>
   </si>
   <si>
@@ -1348,9 +1378,6 @@
     <t xml:space="preserve">Leyla and Adam have had a happy marriage for years. However, after a while, their marriage becomes a dead end. The excitement in their marriage is now gone, and Adam falls into a love that causes his heart to beat again. Adem, who falls in love with the woman named Nergis who comes across this period, cannot think of anyone other than Nergis. However, Nergis, who took the mind of Adam, has no intention of moving to another life from the one-man world he founded.</t>
   </si>
   <si>
-    <t xml:space="preserve">Genres: Comedy</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Turkey </t>
   </si>
   <si>
@@ -1391,7 +1418,7 @@
     <t xml:space="preserve"> Animation, Adventure, Family, Fantasy</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ireland , Luxembourg , France , USA , UK </t>
+    <t xml:space="preserve"> Ireland , Luxembourg , France , Denmark , USA , UK </t>
   </si>
   <si>
     <t xml:space="preserve"> 171,900        
@@ -1532,7 +1559,7 @@
     <t xml:space="preserve"> USA , Canada , Italy </t>
   </si>
   <si>
-    <t xml:space="preserve"> 6,243,740        
+    <t xml:space="preserve"> 6,258,081        
         </t>
   </si>
   <si>
@@ -1625,7 +1652,7 @@
     <t xml:space="preserve">In the skulduggery world of politics and crime, an innocent Chanchal has to put all on the line to prove her innocence and bring justice to Shakti and the people that he loved so much. As she gets embroiled deep in a web of deceit, Chanchal must face powers both natural and supernatural to fulfil her destiny.</t>
   </si>
   <si>
-    <t xml:space="preserve">Genres: Horror, Thriller</t>
+    <t xml:space="preserve"> Horror, Thriller</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1666,6 +1693,9 @@
     <t xml:space="preserve"> agent, female protagonist, </t>
   </si>
   <si>
+    <t xml:space="preserve"> Drama, Music</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dolly Parton's Christmas on the Square</t>
   </si>
   <si>
@@ -1675,6 +1705,9 @@
     <t xml:space="preserve"> christmas, </t>
   </si>
   <si>
+    <t xml:space="preserve"> Comedy, Drama, Family, Musical</t>
+  </si>
+  <si>
     <t xml:space="preserve">
  Magnolia Hill Productions, Sandollar Productions, Warner Bros. Television      
         </t>
@@ -1804,7 +1837,7 @@
     <t xml:space="preserve"> Canada , USA , Portugal </t>
   </si>
   <si>
-    <t xml:space="preserve"> 110,848,357        
+    <t xml:space="preserve"> 110,939,029        
         </t>
   </si>
   <si>
@@ -1863,7 +1896,7 @@
     <t xml:space="preserve"> Drama, Fantasy, Horror</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1,875,405        
+    <t xml:space="preserve"> 1,882,552        
         </t>
   </si>
   <si>
@@ -1898,7 +1931,7 @@
     <t xml:space="preserve">Takes place in 1869, before the events of the original movie. It will finally reveal how the cursed game came to be and the adventures of the first people who played Jumanji.</t>
   </si>
   <si>
-    <t xml:space="preserve">Genres: Adventure</t>
+    <t xml:space="preserve"> Adventure</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1977,7 +2010,7 @@
     <t xml:space="preserve">The Dark and The Wicked follows two siblings who are summoned back to the family farm to await the inevitability of their father's death. What initially appears to be a timeless ritual of loss and remembrance turns out to be something very different.</t>
   </si>
   <si>
-    <t xml:space="preserve">Genres: Horror</t>
+    <t xml:space="preserve"> Horror</t>
   </si>
   <si>
     <t xml:space="preserve"> 334,022        
@@ -2018,6 +2051,9 @@
     <t xml:space="preserve"> survival, </t>
   </si>
   <si>
+    <t xml:space="preserve"> Action</t>
+  </si>
+  <si>
     <t xml:space="preserve"> China </t>
   </si>
   <si>
@@ -2036,7 +2072,7 @@
     <t xml:space="preserve">A man rises from personal tragedy to lead a group of children from a refugee camp to victory, transforming their lives through the game of cricket.</t>
   </si>
   <si>
-    <t xml:space="preserve">Genres: Action, Drama, Sport, Thriller</t>
+    <t xml:space="preserve"> Action, Drama, Sport, Thriller</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -2058,21 +2094,26 @@
         </t>
   </si>
   <si>
-    <t xml:space="preserve">Peninsula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peninsula takes place four years after the zombie outbreak in Train to Busan. The Korean peninsula is devastated and Jung Seok, a former soldier who has managed to escape overseas, is given a mission to go back and unexpectedly meets survivors.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> zombie, zombie apocalypse, united nations blue helmet, sequel, second part, </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 39,521,135        
-        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- Next Entertainment World, RedPeter Film      
+    <t xml:space="preserve">Free Guy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A bank teller discovers that he's actually an NPC inside a brutal, open world video game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bank robbery, gamers, two word title, virtual reality, heroic, </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Action, Adventure, Comedy, Sci-Fi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> USA , Canada , Japan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 20th Century Studios, 21 Laps Entertainment, Berlanti Productions      
         </t>
   </si>
 </sst>
@@ -2590,810 +2631,826 @@
       <c r="D7" t="s">
         <v>50</v>
       </c>
-      <c r="E7"/>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" t="s">
         <v>70</v>
       </c>
-      <c r="E10"/>
+      <c r="D10"/>
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G10"/>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F12" t="s">
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
         <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14"/>
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
       <c r="F14" t="s">
         <v>22</v>
       </c>
       <c r="G14"/>
       <c r="H14" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I14" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E15" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F15" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H15" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I15" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
-      </c>
-      <c r="E16"/>
+        <v>111</v>
+      </c>
+      <c r="E16" t="s">
+        <v>112</v>
+      </c>
       <c r="F16" t="s">
         <v>22</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I16" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
-        <v>113</v>
-      </c>
-      <c r="E17"/>
+        <v>116</v>
+      </c>
+      <c r="E17" t="s">
+        <v>117</v>
+      </c>
       <c r="F17" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="G17" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="H17" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="I17" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D18" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E18" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
       </c>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="I18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D19" t="s">
-        <v>125</v>
-      </c>
-      <c r="E19"/>
+        <v>129</v>
+      </c>
+      <c r="E19" t="s">
+        <v>130</v>
+      </c>
       <c r="F19" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="G19"/>
       <c r="H19" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="I19" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F20" t="s">
         <v>22</v>
       </c>
       <c r="G20"/>
       <c r="H20" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="I20" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D21" t="s">
-        <v>137</v>
-      </c>
-      <c r="E21"/>
+        <v>142</v>
+      </c>
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
       <c r="F21" t="s">
         <v>22</v>
       </c>
       <c r="G21"/>
       <c r="H21" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="I21" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D22" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="E22" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G22" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="H22" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="I22" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D23" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E23" t="s">
         <v>44</v>
       </c>
       <c r="F23" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="G23" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="H23" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="I23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D24" t="s">
-        <v>155</v>
-      </c>
-      <c r="E24"/>
+        <v>160</v>
+      </c>
+      <c r="E24" t="s">
+        <v>161</v>
+      </c>
       <c r="F24" t="s">
         <v>22</v>
       </c>
       <c r="G24"/>
       <c r="H24" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="I24" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D25" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E25" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="F25" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="G25"/>
       <c r="H25" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="I25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D26" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F26" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="G26" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="H26" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="I26" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D27" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="E27" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F27" t="s">
         <v>22</v>
       </c>
       <c r="G27"/>
       <c r="H27" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="I27" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D28" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="E28" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F28" t="s">
         <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="H28" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="I28" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="D29" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="E29" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="F29" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="G29" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="H29" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="I29" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
       </c>
       <c r="C30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D30" t="s">
+        <v>199</v>
+      </c>
+      <c r="E30" t="s">
         <v>192</v>
-      </c>
-      <c r="D30" t="s">
-        <v>193</v>
-      </c>
-      <c r="E30" t="s">
-        <v>186</v>
       </c>
       <c r="F30" t="s">
         <v>22</v>
       </c>
       <c r="G30" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="H30" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="I30" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D31" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="E31" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F31" t="s">
         <v>22</v>
       </c>
       <c r="G31" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="H31" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="I31" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>204</v>
-      </c>
-      <c r="D32" t="s">
-        <v>205</v>
-      </c>
-      <c r="E32"/>
+        <v>210</v>
+      </c>
+      <c r="D32"/>
+      <c r="E32" t="s">
+        <v>211</v>
+      </c>
       <c r="F32" t="s">
         <v>22</v>
       </c>
       <c r="G32"/>
       <c r="H32" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="I32" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="D33" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="E33" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="F33" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="G33" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="H33" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="I33" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="D34" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E34" t="s">
-        <v>219</v>
+        <v>71</v>
       </c>
       <c r="F34" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="G34" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="H34" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="I34" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="D35" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="E35" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F35" t="s">
         <v>22</v>
       </c>
       <c r="G35" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="H35" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="I35" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="D36" t="s">
-        <v>232</v>
-      </c>
-      <c r="E36"/>
+        <v>237</v>
+      </c>
+      <c r="E36" t="s">
+        <v>238</v>
+      </c>
       <c r="F36" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="G36"/>
       <c r="H36" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="I36" t="s">
         <v>25</v>
@@ -3401,576 +3458,584 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="D37" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="E37" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="F37" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="G37" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="H37" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="I37" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="D38" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="E38" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="F38" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="G38"/>
       <c r="H38" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="I38" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="D39" t="s">
-        <v>250</v>
-      </c>
-      <c r="E39"/>
+        <v>256</v>
+      </c>
+      <c r="E39" t="s">
+        <v>192</v>
+      </c>
       <c r="F39" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G39" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="H39" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="I39" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="D40" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="E40" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="F40" t="s">
         <v>22</v>
       </c>
       <c r="G40"/>
       <c r="H40" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="I40" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="D41" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="E41" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="F41" t="s">
         <v>22</v>
       </c>
       <c r="G41"/>
       <c r="H41" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="I41" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="D42" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="E42" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="F42" t="s">
         <v>22</v>
       </c>
       <c r="G42" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="H42" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="I42" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B43" t="s">
         <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="D43" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="E43" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="F43" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="G43" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="H43" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="I43" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="D44" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="E44" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F44" t="s">
         <v>22</v>
       </c>
       <c r="G44"/>
       <c r="H44" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="I44" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="D45" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="E45" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="F45" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="G45"/>
       <c r="H45" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="I45" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="D46" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="E46" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="F46" t="s">
         <v>22</v>
       </c>
       <c r="G46" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="H46" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="I46" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="B47" t="s">
         <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="D47" t="s">
-        <v>296</v>
-      </c>
-      <c r="E47"/>
+        <v>302</v>
+      </c>
+      <c r="E47" t="s">
+        <v>303</v>
+      </c>
       <c r="F47" t="s">
         <v>22</v>
       </c>
       <c r="G47" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="H47" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="I47" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="D48" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="E48" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="F48" t="s">
         <v>22</v>
       </c>
       <c r="G48"/>
       <c r="H48" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="I48"/>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="B49" t="s">
         <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="D49" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="E49" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="F49" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="G49" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="H49" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="I49" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="D50" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="E50" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="F50" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="G50" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="H50" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="I50" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="B51" t="s">
         <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="D51" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="E51" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="F51" t="s">
         <v>22</v>
       </c>
       <c r="G51" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="H51" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="I51" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="D52" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="E52" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="F52" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="G52" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="H52" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="I52" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="B53" t="s">
         <v>10</v>
       </c>
       <c r="C53" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="D53" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="E53" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="F53" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="G53"/>
       <c r="H53" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="I53" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="B54" t="s">
         <v>10</v>
       </c>
       <c r="C54" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="D54" t="s">
-        <v>342</v>
-      </c>
-      <c r="E54"/>
+        <v>349</v>
+      </c>
+      <c r="E54" t="s">
+        <v>192</v>
+      </c>
       <c r="F54" t="s">
         <v>22</v>
       </c>
       <c r="G54"/>
       <c r="H54" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="I54" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="B55" t="s">
         <v>10</v>
       </c>
       <c r="C55" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="D55" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="E55" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="F55" t="s">
         <v>22</v>
       </c>
       <c r="G55"/>
       <c r="H55" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="I55" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="D56" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="E56" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="F56" t="s">
         <v>14</v>
       </c>
       <c r="G56"/>
       <c r="H56" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="I56" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="D57" t="s">
-        <v>356</v>
-      </c>
-      <c r="E57"/>
+        <v>363</v>
+      </c>
+      <c r="E57" t="s">
+        <v>364</v>
+      </c>
       <c r="F57" t="s">
         <v>22</v>
       </c>
       <c r="G57"/>
       <c r="H57" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="I57" t="s">
         <v>40</v>
@@ -3978,346 +4043,350 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="B58" t="s">
         <v>10</v>
       </c>
       <c r="C58" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="D58" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="E58" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
       <c r="F58" t="s">
         <v>22</v>
       </c>
       <c r="G58"/>
       <c r="H58" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="I58" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="B59" t="s">
         <v>10</v>
       </c>
       <c r="C59" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
       <c r="D59" t="s">
-        <v>366</v>
-      </c>
-      <c r="E59"/>
+        <v>374</v>
+      </c>
+      <c r="E59" t="s">
+        <v>375</v>
+      </c>
       <c r="F59" t="s">
         <v>22</v>
       </c>
       <c r="G59" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="H59" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="I59" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
       </c>
       <c r="C60" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="D60" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="E60" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="F60" t="s">
         <v>22</v>
       </c>
       <c r="G60" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="H60" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="I60" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="B61" t="s">
         <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="D61" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="E61" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="F61" t="s">
         <v>22</v>
       </c>
       <c r="G61"/>
       <c r="H61" t="s">
-        <v>379</v>
-      </c>
-      <c r="I61"/>
+        <v>388</v>
+      </c>
+      <c r="I61" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="D62" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="E62" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="F62" t="s">
         <v>14</v>
       </c>
       <c r="G62"/>
       <c r="H62" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="I62" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="B63" t="s">
         <v>10</v>
       </c>
       <c r="C63" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="D63" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="E63" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="F63" t="s">
         <v>22</v>
       </c>
       <c r="G63"/>
       <c r="H63" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="I63" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="B64" t="s">
         <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>392</v>
-      </c>
-      <c r="D64" t="s">
-        <v>393</v>
-      </c>
-      <c r="E64"/>
+        <v>402</v>
+      </c>
+      <c r="D64"/>
+      <c r="E64" t="s">
+        <v>359</v>
+      </c>
       <c r="F64" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="G64"/>
       <c r="H64" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="I64" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="B65" t="s">
         <v>10</v>
       </c>
       <c r="C65" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="D65" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="E65" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="F65" t="s">
         <v>22</v>
       </c>
       <c r="G65"/>
       <c r="H65" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="I65" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="B66" t="s">
         <v>10</v>
       </c>
       <c r="C66" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="D66" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="E66" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="F66" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="G66" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
       <c r="H66" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="I66" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="B67" t="s">
         <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="D67" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="E67" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="F67" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="G67" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="H67" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="I67" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="D68" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="E68" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="F68" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="G68" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
       <c r="H68" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="I68" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="D69" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
       <c r="E69" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
       <c r="F69" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="G69" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="H69" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="I69" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="B70" t="s">
         <v>10</v>
       </c>
       <c r="C70" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="D70" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
@@ -4326,249 +4395,251 @@
         <v>22</v>
       </c>
       <c r="G70" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="H70" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="I70" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="B71" t="s">
         <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
       <c r="D71" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="E71" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
       <c r="F71" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="G71" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
       <c r="H71" t="s">
-        <v>441</v>
+        <v>450</v>
       </c>
       <c r="I71" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
       <c r="B72" t="s">
         <v>10</v>
       </c>
       <c r="C72" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="D72" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="E72" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="F72" t="s">
-        <v>446</v>
+        <v>455</v>
       </c>
       <c r="G72" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="H72" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
       <c r="I72" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
       <c r="B73" t="s">
         <v>10</v>
       </c>
       <c r="C73" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="D73" t="s">
-        <v>452</v>
+        <v>461</v>
       </c>
       <c r="E73" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
       <c r="F73" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="G73"/>
       <c r="H73" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
       <c r="I73"/>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>456</v>
+        <v>465</v>
       </c>
       <c r="B74" t="s">
         <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
       <c r="D74" t="s">
-        <v>458</v>
+        <v>467</v>
       </c>
       <c r="E74" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
       <c r="F74" t="s">
         <v>22</v>
       </c>
       <c r="G74"/>
       <c r="H74" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="I74" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="B75" t="s">
         <v>10</v>
       </c>
       <c r="C75" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
       <c r="D75" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
       <c r="E75" t="s">
         <v>37</v>
       </c>
       <c r="F75" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="G75"/>
       <c r="H75" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
       <c r="I75" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
       <c r="B76" t="s">
         <v>10</v>
       </c>
       <c r="C76" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
       <c r="D76" t="s">
-        <v>468</v>
+        <v>477</v>
       </c>
       <c r="E76" t="s">
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="F76" t="s">
         <v>22</v>
       </c>
       <c r="G76" t="s">
-        <v>470</v>
+        <v>479</v>
       </c>
       <c r="H76" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
       <c r="I76" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
       <c r="B77" t="s">
         <v>10</v>
       </c>
       <c r="C77" t="s">
-        <v>473</v>
-      </c>
-      <c r="D77" t="s">
-        <v>474</v>
-      </c>
-      <c r="E77"/>
+        <v>482</v>
+      </c>
+      <c r="D77"/>
+      <c r="E77" t="s">
+        <v>483</v>
+      </c>
       <c r="F77" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="G77"/>
       <c r="H77" t="s">
-        <v>475</v>
+        <v>484</v>
       </c>
       <c r="I77" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
       <c r="B78" t="s">
         <v>10</v>
       </c>
       <c r="C78" t="s">
-        <v>478</v>
+        <v>487</v>
       </c>
       <c r="D78" t="s">
-        <v>479</v>
+        <v>488</v>
       </c>
       <c r="E78" t="s">
-        <v>480</v>
+        <v>489</v>
       </c>
       <c r="F78" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="G78" t="s">
-        <v>481</v>
+        <v>490</v>
       </c>
       <c r="H78" t="s">
-        <v>482</v>
+        <v>491</v>
       </c>
       <c r="I78" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="B79" t="s">
         <v>10</v>
       </c>
       <c r="C79" t="s">
-        <v>484</v>
+        <v>493</v>
       </c>
       <c r="D79" t="s">
-        <v>485</v>
-      </c>
-      <c r="E79"/>
+        <v>494</v>
+      </c>
+      <c r="E79" t="s">
+        <v>495</v>
+      </c>
       <c r="F79" t="s">
         <v>22</v>
       </c>
@@ -4577,598 +4648,604 @@
         <v>24</v>
       </c>
       <c r="I79" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>486</v>
+        <v>496</v>
       </c>
       <c r="B80" t="s">
         <v>10</v>
       </c>
       <c r="C80" t="s">
-        <v>487</v>
+        <v>497</v>
       </c>
       <c r="D80" t="s">
-        <v>488</v>
-      </c>
-      <c r="E80"/>
+        <v>498</v>
+      </c>
+      <c r="E80" t="s">
+        <v>499</v>
+      </c>
       <c r="F80" t="s">
         <v>22</v>
       </c>
       <c r="G80"/>
       <c r="H80" t="s">
-        <v>489</v>
+        <v>500</v>
       </c>
       <c r="I80" t="s">
-        <v>490</v>
+        <v>501</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>491</v>
+        <v>502</v>
       </c>
       <c r="B81" t="s">
         <v>10</v>
       </c>
       <c r="C81" t="s">
-        <v>492</v>
+        <v>503</v>
       </c>
       <c r="D81" t="s">
-        <v>493</v>
+        <v>504</v>
       </c>
       <c r="E81" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F81" t="s">
         <v>22</v>
       </c>
       <c r="G81" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="H81" t="s">
-        <v>495</v>
+        <v>506</v>
       </c>
       <c r="I81" t="s">
-        <v>496</v>
+        <v>507</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>497</v>
+        <v>508</v>
       </c>
       <c r="B82" t="s">
         <v>10</v>
       </c>
       <c r="C82" t="s">
-        <v>498</v>
+        <v>509</v>
       </c>
       <c r="D82" t="s">
-        <v>499</v>
+        <v>510</v>
       </c>
       <c r="E82" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F82" t="s">
-        <v>500</v>
+        <v>511</v>
       </c>
       <c r="G82"/>
       <c r="H82" t="s">
-        <v>501</v>
+        <v>512</v>
       </c>
       <c r="I82" t="s">
-        <v>502</v>
+        <v>513</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>503</v>
+        <v>514</v>
       </c>
       <c r="B83" t="s">
         <v>10</v>
       </c>
       <c r="C83" t="s">
-        <v>504</v>
+        <v>515</v>
       </c>
       <c r="D83" t="s">
-        <v>505</v>
+        <v>516</v>
       </c>
       <c r="E83" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="F83" t="s">
         <v>22</v>
       </c>
       <c r="G83"/>
       <c r="H83" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="I83" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>507</v>
+        <v>518</v>
       </c>
       <c r="B84" t="s">
         <v>10</v>
       </c>
       <c r="C84" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="D84" t="s">
-        <v>509</v>
+        <v>520</v>
       </c>
       <c r="E84" t="s">
-        <v>510</v>
+        <v>521</v>
       </c>
       <c r="F84" t="s">
-        <v>511</v>
+        <v>522</v>
       </c>
       <c r="G84"/>
       <c r="H84" t="s">
-        <v>512</v>
+        <v>523</v>
       </c>
       <c r="I84" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>513</v>
+        <v>524</v>
       </c>
       <c r="B85" t="s">
         <v>10</v>
       </c>
       <c r="C85" t="s">
-        <v>514</v>
+        <v>525</v>
       </c>
       <c r="D85" t="s">
-        <v>515</v>
+        <v>526</v>
       </c>
       <c r="E85" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F85" t="s">
-        <v>516</v>
+        <v>527</v>
       </c>
       <c r="G85"/>
       <c r="H85" t="s">
-        <v>517</v>
+        <v>528</v>
       </c>
       <c r="I85" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>518</v>
+        <v>529</v>
       </c>
       <c r="B86" t="s">
         <v>10</v>
       </c>
       <c r="C86" t="s">
-        <v>519</v>
+        <v>530</v>
       </c>
       <c r="D86" t="s">
-        <v>520</v>
-      </c>
-      <c r="E86"/>
+        <v>531</v>
+      </c>
+      <c r="E86" t="s">
+        <v>91</v>
+      </c>
       <c r="F86" t="s">
         <v>22</v>
       </c>
       <c r="G86"/>
       <c r="H86" t="s">
-        <v>521</v>
+        <v>532</v>
       </c>
       <c r="I86" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>522</v>
+        <v>533</v>
       </c>
       <c r="B87" t="s">
         <v>10</v>
       </c>
       <c r="C87" t="s">
-        <v>523</v>
+        <v>534</v>
       </c>
       <c r="D87" t="s">
-        <v>524</v>
+        <v>535</v>
       </c>
       <c r="E87" t="s">
-        <v>525</v>
+        <v>536</v>
       </c>
       <c r="F87" t="s">
-        <v>526</v>
+        <v>537</v>
       </c>
       <c r="G87" t="s">
-        <v>527</v>
+        <v>538</v>
       </c>
       <c r="H87" t="s">
-        <v>528</v>
+        <v>539</v>
       </c>
       <c r="I87" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>529</v>
+        <v>540</v>
       </c>
       <c r="B88" t="s">
         <v>10</v>
       </c>
       <c r="C88" t="s">
-        <v>530</v>
+        <v>541</v>
       </c>
       <c r="D88" t="s">
-        <v>531</v>
+        <v>542</v>
       </c>
       <c r="E88" t="s">
-        <v>532</v>
+        <v>543</v>
       </c>
       <c r="F88" t="s">
-        <v>533</v>
+        <v>544</v>
       </c>
       <c r="G88" t="s">
-        <v>534</v>
+        <v>545</v>
       </c>
       <c r="H88" t="s">
-        <v>535</v>
+        <v>546</v>
       </c>
       <c r="I88" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>536</v>
+        <v>547</v>
       </c>
       <c r="B89" t="s">
         <v>10</v>
       </c>
       <c r="C89" t="s">
-        <v>537</v>
+        <v>548</v>
       </c>
       <c r="D89" t="s">
-        <v>538</v>
-      </c>
-      <c r="E89"/>
+        <v>549</v>
+      </c>
+      <c r="E89" t="s">
+        <v>130</v>
+      </c>
       <c r="F89" t="s">
         <v>22</v>
       </c>
       <c r="G89"/>
       <c r="H89" t="s">
-        <v>539</v>
+        <v>550</v>
       </c>
       <c r="I89"/>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>540</v>
+        <v>551</v>
       </c>
       <c r="B90" t="s">
         <v>10</v>
       </c>
       <c r="C90" t="s">
-        <v>541</v>
+        <v>552</v>
       </c>
       <c r="D90" t="s">
-        <v>542</v>
+        <v>553</v>
       </c>
       <c r="E90" t="s">
-        <v>543</v>
+        <v>554</v>
       </c>
       <c r="F90" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G90" t="s">
-        <v>544</v>
+        <v>555</v>
       </c>
       <c r="H90" t="s">
-        <v>545</v>
+        <v>556</v>
       </c>
       <c r="I90" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>546</v>
+        <v>557</v>
       </c>
       <c r="B91" t="s">
         <v>10</v>
       </c>
       <c r="C91" t="s">
-        <v>547</v>
+        <v>558</v>
       </c>
       <c r="D91" t="s">
-        <v>548</v>
+        <v>559</v>
       </c>
       <c r="E91" t="s">
-        <v>549</v>
+        <v>560</v>
       </c>
       <c r="F91" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="G91"/>
       <c r="H91" t="s">
-        <v>551</v>
+        <v>562</v>
       </c>
       <c r="I91" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>552</v>
+        <v>563</v>
       </c>
       <c r="B92" t="s">
         <v>10</v>
       </c>
       <c r="C92" t="s">
-        <v>553</v>
-      </c>
-      <c r="D92" t="s">
-        <v>554</v>
-      </c>
-      <c r="E92"/>
+        <v>564</v>
+      </c>
+      <c r="D92"/>
+      <c r="E92" t="s">
+        <v>565</v>
+      </c>
       <c r="F92" t="s">
         <v>22</v>
       </c>
       <c r="G92"/>
       <c r="H92" t="s">
-        <v>555</v>
+        <v>566</v>
       </c>
       <c r="I92"/>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>556</v>
+        <v>567</v>
       </c>
       <c r="B93" t="s">
         <v>10</v>
       </c>
       <c r="C93" t="s">
-        <v>557</v>
+        <v>568</v>
       </c>
       <c r="D93" t="s">
-        <v>558</v>
+        <v>569</v>
       </c>
       <c r="E93" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="F93" t="s">
-        <v>559</v>
+        <v>570</v>
       </c>
       <c r="G93"/>
       <c r="H93" t="s">
-        <v>560</v>
+        <v>571</v>
       </c>
       <c r="I93" t="s">
-        <v>561</v>
+        <v>572</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>562</v>
+        <v>573</v>
       </c>
       <c r="B94" t="s">
         <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>563</v>
+        <v>574</v>
       </c>
       <c r="D94" t="s">
-        <v>564</v>
+        <v>575</v>
       </c>
       <c r="E94" t="s">
-        <v>565</v>
+        <v>576</v>
       </c>
       <c r="F94" t="s">
-        <v>566</v>
+        <v>577</v>
       </c>
       <c r="G94" t="s">
-        <v>567</v>
+        <v>578</v>
       </c>
       <c r="H94" t="s">
-        <v>568</v>
+        <v>579</v>
       </c>
       <c r="I94" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>569</v>
+        <v>580</v>
       </c>
       <c r="B95" t="s">
         <v>10</v>
       </c>
       <c r="C95" t="s">
-        <v>570</v>
+        <v>581</v>
       </c>
       <c r="D95" t="s">
-        <v>571</v>
+        <v>582</v>
       </c>
       <c r="E95" t="s">
-        <v>572</v>
+        <v>583</v>
       </c>
       <c r="F95" t="s">
         <v>22</v>
       </c>
       <c r="G95" t="s">
-        <v>573</v>
+        <v>584</v>
       </c>
       <c r="H95" t="s">
-        <v>574</v>
+        <v>585</v>
       </c>
       <c r="I95" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>575</v>
+        <v>586</v>
       </c>
       <c r="B96" t="s">
         <v>10</v>
       </c>
       <c r="C96" t="s">
-        <v>576</v>
-      </c>
-      <c r="D96" t="s">
-        <v>577</v>
-      </c>
-      <c r="E96"/>
+        <v>587</v>
+      </c>
+      <c r="D96"/>
+      <c r="E96" t="s">
+        <v>588</v>
+      </c>
       <c r="F96" t="s">
         <v>22</v>
       </c>
       <c r="G96" t="s">
-        <v>578</v>
+        <v>589</v>
       </c>
       <c r="H96" t="s">
-        <v>579</v>
+        <v>590</v>
       </c>
       <c r="I96" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>580</v>
+        <v>591</v>
       </c>
       <c r="B97" t="s">
         <v>10</v>
       </c>
       <c r="C97" t="s">
-        <v>581</v>
+        <v>592</v>
       </c>
       <c r="D97" t="s">
-        <v>582</v>
+        <v>593</v>
       </c>
       <c r="E97" t="s">
-        <v>583</v>
+        <v>594</v>
       </c>
       <c r="F97" t="s">
-        <v>584</v>
+        <v>595</v>
       </c>
       <c r="G97"/>
       <c r="H97" t="s">
-        <v>585</v>
+        <v>596</v>
       </c>
       <c r="I97" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>586</v>
+        <v>597</v>
       </c>
       <c r="B98" t="s">
         <v>10</v>
       </c>
       <c r="C98" t="s">
-        <v>587</v>
+        <v>598</v>
       </c>
       <c r="D98" t="s">
-        <v>588</v>
-      </c>
-      <c r="E98"/>
+        <v>599</v>
+      </c>
+      <c r="E98" t="s">
+        <v>600</v>
+      </c>
       <c r="F98" t="s">
-        <v>589</v>
+        <v>601</v>
       </c>
       <c r="G98" t="s">
-        <v>590</v>
+        <v>602</v>
       </c>
       <c r="H98" t="s">
-        <v>591</v>
+        <v>603</v>
       </c>
       <c r="I98" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>592</v>
+        <v>604</v>
       </c>
       <c r="B99" t="s">
         <v>10</v>
       </c>
       <c r="C99" t="s">
-        <v>593</v>
-      </c>
-      <c r="D99" t="s">
-        <v>594</v>
-      </c>
-      <c r="E99"/>
+        <v>605</v>
+      </c>
+      <c r="D99"/>
+      <c r="E99" t="s">
+        <v>606</v>
+      </c>
       <c r="F99" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="G99"/>
       <c r="H99" t="s">
-        <v>595</v>
+        <v>607</v>
       </c>
       <c r="I99"/>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>596</v>
+        <v>608</v>
       </c>
       <c r="B100" t="s">
         <v>10</v>
       </c>
       <c r="C100" t="s">
-        <v>597</v>
+        <v>609</v>
       </c>
       <c r="D100" t="s">
-        <v>598</v>
-      </c>
-      <c r="E100"/>
+        <v>610</v>
+      </c>
+      <c r="E100" t="s">
+        <v>335</v>
+      </c>
       <c r="F100" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="G100"/>
       <c r="H100" t="s">
-        <v>599</v>
+        <v>611</v>
       </c>
       <c r="I100" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>600</v>
+        <v>612</v>
       </c>
       <c r="B101" t="s">
-        <v>10</v>
+        <v>613</v>
       </c>
       <c r="C101" t="s">
-        <v>601</v>
+        <v>614</v>
       </c>
       <c r="D101" t="s">
-        <v>602</v>
+        <v>615</v>
       </c>
       <c r="E101" t="s">
-        <v>307</v>
+        <v>616</v>
       </c>
       <c r="F101" t="s">
-        <v>161</v>
-      </c>
-      <c r="G101" t="s">
-        <v>603</v>
-      </c>
+        <v>617</v>
+      </c>
+      <c r="G101"/>
       <c r="H101" t="s">
-        <v>604</v>
-      </c>
-      <c r="I101" t="s">
-        <v>93</v>
-      </c>
+        <v>618</v>
+      </c>
+      <c r="I101"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>